<commit_message>
added parserFE + vanilla results.
</commit_message>
<xml_diff>
--- a/experiments/220_asr/220_results.xlsx
+++ b/experiments/220_asr/220_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20440" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="9120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Overall performance</t>
   </si>
@@ -56,18 +56,45 @@
   <si>
     <t>CRF + VanillaFE (window size 4)</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Measuremen</t>
+  </si>
+  <si>
+    <t>Token Prec</t>
+  </si>
+  <si>
+    <t>Token Rec</t>
+  </si>
+  <si>
+    <t>Token F1</t>
+  </si>
+  <si>
+    <t>Span Pr</t>
+  </si>
+  <si>
+    <t>Span Re</t>
+  </si>
+  <si>
+    <t>Span F1</t>
+  </si>
+  <si>
+    <t>CRF 10F</t>
+  </si>
+  <si>
+    <t>vanilla w=4</t>
+  </si>
+  <si>
+    <t>parserFE w=2</t>
+  </si>
+  <si>
+    <t>220 files</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -437,19 +464,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26">
+    <row r="4" spans="1:7" ht="38.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +501,7 @@
         <v>0.45617021276595698</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -495,7 +524,7 @@
         <v>0.48054919908466798</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26">
+    <row r="6" spans="1:7" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -518,7 +547,7 @@
         <v>0.484969939879759</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26">
+    <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -541,7 +570,7 @@
         <v>0.50980392156862697</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26">
+    <row r="8" spans="1:7" ht="25.5">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -564,7 +593,7 @@
         <v>0.396039603960396</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26">
+    <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -587,7 +616,7 @@
         <v>0.47495361781076001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26">
+    <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -610,7 +639,7 @@
         <v>0.48290598290598202</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26">
+    <row r="11" spans="1:7" ht="25.5">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -633,7 +662,7 @@
         <v>0.40816326530612201</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26">
+    <row r="12" spans="1:7" ht="25.5">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -656,7 +685,7 @@
         <v>0.45822102425875999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26">
+    <row r="13" spans="1:7" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -679,7 +708,7 @@
         <v>0.420382165605095</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26">
+    <row r="14" spans="1:7" ht="25.5">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -700,12 +729,304 @@
       </c>
       <c r="G14" s="1">
         <v>0.43722943722943702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="38.25">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.78876678876678796</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.39868339847767897</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.52965291063131903</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.68971848225214105</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.37170184696569902</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.483069009858551</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="25.5">
+      <c r="A24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.810276679841897</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.42797494780793299</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.56010928961748596</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.50655021834061098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="25.5">
+      <c r="A25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.76785714285714202</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.43877551020408101</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.55844155844155796</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.60526315789473595</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.40780141843971601</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.48728813559321998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="25.5">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.843537414965986</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.41891891891891803</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.55981941309255001</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.37765957446808501</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.49305555555555503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="25.5">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.75675675675675602</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.68531468531468498</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.53405994550408697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="25.5">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.82033898305084696</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.456603773584905</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.586666666666666</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.75647668393782297</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.47096774193548302</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.58051689860834899</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="25.5">
+      <c r="A29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.77104377104377098</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.41335740072202098</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.53819036427732003</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.71052631578947301</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.38793103448275801</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.50185873605947895</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="25.5">
+      <c r="A30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.84523809523809501</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.41846758349705299</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.55978975032851497</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.77272727272727204</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.38746438746438699</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.51612903225806395</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="25.5">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.81140350877192902</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.35238095238095202</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.49136786188579001</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.69444444444444398</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.32051282051281998</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.43859649122806998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="25.5">
+      <c r="A32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.26844583987441101</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.39537572254335202</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.61783439490445802</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.234866828087167</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.34035087719298202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="25.5">
+      <c r="A33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.72941176470588198</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.40172786177105801</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.51810584958217198</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.65317919075144504</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.35987261146496802</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.464065708418891</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add results for 220 asr using phoneFE only
</commit_message>
<xml_diff>
--- a/experiments/220_asr/220_results.xlsx
+++ b/experiments/220_asr/220_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="15480" windowHeight="9120" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="20280" windowHeight="14260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Overall performance</t>
   </si>
@@ -54,10 +54,6 @@
     <t>Test partition 9</t>
   </si>
   <si>
-    <t>CRF + VanillaFE (window size 4)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Measuremen</t>
   </si>
   <si>
@@ -88,15 +84,31 @@
     <t>parserFE w=2</t>
   </si>
   <si>
-    <t>220 files</t>
+    <t>CRF PhoneFE unigram, no currentSpan, with phoneTypes and phoneTypePatterns</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRF VanillaFE (window size 4)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -130,11 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -464,21 +477,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="38.25">
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="26">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +537,7 @@
         <v>0.45617021276595698</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="25.5">
+    <row r="5" spans="1:7" ht="26">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -524,7 +560,7 @@
         <v>0.48054919908466798</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="25.5">
+    <row r="6" spans="1:7" ht="26">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -547,7 +583,7 @@
         <v>0.484969939879759</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
+    <row r="7" spans="1:7" ht="26">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -570,7 +606,7 @@
         <v>0.50980392156862697</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="25.5">
+    <row r="8" spans="1:7" ht="26">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -593,7 +629,7 @@
         <v>0.396039603960396</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="25.5">
+    <row r="9" spans="1:7" ht="26">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -616,7 +652,7 @@
         <v>0.47495361781076001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="25.5">
+    <row r="10" spans="1:7" ht="26">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -639,7 +675,7 @@
         <v>0.48290598290598202</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="25.5">
+    <row r="11" spans="1:7" ht="26">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -662,7 +698,7 @@
         <v>0.40816326530612201</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="25.5">
+    <row r="12" spans="1:7" ht="26">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -685,7 +721,7 @@
         <v>0.45822102425875999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="25.5">
+    <row r="13" spans="1:7" ht="26">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -708,7 +744,7 @@
         <v>0.420382165605095</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="25.5">
+    <row r="14" spans="1:7" ht="26">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -731,46 +767,18 @@
         <v>0.43722943722943702</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="2" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="38.25">
+    </row>
+    <row r="23" spans="1:7" ht="26">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,7 +801,7 @@
         <v>0.483069009858551</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="25.5">
+    <row r="24" spans="1:7" ht="26">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -816,7 +824,7 @@
         <v>0.50655021834061098</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="25.5">
+    <row r="25" spans="1:7" ht="26">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -839,7 +847,7 @@
         <v>0.48728813559321998</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="25.5">
+    <row r="26" spans="1:7" ht="26">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -862,7 +870,7 @@
         <v>0.49305555555555503</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="25.5">
+    <row r="27" spans="1:7" ht="26">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -885,7 +893,7 @@
         <v>0.53405994550408697</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="25.5">
+    <row r="28" spans="1:7" ht="26">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -908,7 +916,7 @@
         <v>0.58051689860834899</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="25.5">
+    <row r="29" spans="1:7" ht="26">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -931,7 +939,7 @@
         <v>0.50185873605947895</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="25.5">
+    <row r="30" spans="1:7" ht="26">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -954,7 +962,7 @@
         <v>0.51612903225806395</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="25.5">
+    <row r="31" spans="1:7" ht="26">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -977,7 +985,7 @@
         <v>0.43859649122806998</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="25.5">
+    <row r="32" spans="1:7" ht="26">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -1000,7 +1008,7 @@
         <v>0.34035087719298202</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="25.5">
+    <row r="33" spans="1:7" ht="26">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1023,10 +1031,268 @@
         <v>0.464065708418891</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="26">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.52798053527980504</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.13392306109853899</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.21365277321956</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.38250428816466497</v>
+      </c>
+      <c r="F37" s="1">
+        <v>7.3548812664907606E-2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.12337482710926601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="26">
+      <c r="A38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.55405405405405395</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.19967532467532401</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.29355608591885402</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.396039603960396</v>
+      </c>
+      <c r="F38" s="1">
+        <v>9.8765432098765399E-2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.158102766798418</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="26">
+      <c r="A39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="C39" s="1">
+        <v>7.0796460176991094E-2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.122137404580152</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.314285714285714</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>9.3617021276595699E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="26">
+      <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="C40" s="1">
+        <v>8.6393088552915706E-2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.145985401459854</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="F40" s="1">
+        <v>4.7058823529411702E-2</v>
+      </c>
+      <c r="G40" s="1">
+        <v>8.16326530612244E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="26">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.487179487179487</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.112759643916913</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.183132530120481</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.32432432432432401</v>
+      </c>
+      <c r="F41" s="1">
+        <v>5.7142857142857099E-2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>9.7165991902833995E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="26">
+      <c r="A42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.51633986928104503</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.22832369942196501</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.316633266533066</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.413333333333333</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0.12704918032786799</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0.194357366771159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="26">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.141666666666666</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.22479338842975199</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.40677966101694901</v>
+      </c>
+      <c r="F43" s="1">
+        <v>7.8175895765472306E-2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0.13114754098360601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="26">
+      <c r="A44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.45871559633027498</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.120481927710843</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.19083969465648801</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.35849056603773499</v>
+      </c>
+      <c r="F44" s="1">
+        <v>6.6433566433566404E-2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>0.112094395280236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="26">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.66386554621848703</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.14522058823529399</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.23831070889894401</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.41071428571428498</v>
+      </c>
+      <c r="F45" s="1">
+        <v>6.9069069069068997E-2</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.118251928020565</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="26">
+      <c r="A46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.47435897435897401</v>
+      </c>
+      <c r="C46" s="1">
+        <v>8.3900226757369606E-2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.14258188824662801</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3.6290322580645101E-2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>6.4056939501779306E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="26">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.56818181818181801</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.138121546961325</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.51724137931034397</v>
+      </c>
+      <c r="F47" s="1">
+        <v>8.9820359281437098E-2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>0.15306122448979501</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added all features results.. seems to be nice with recall
</commit_message>
<xml_diff>
--- a/experiments/220_asr/220_results.xlsx
+++ b/experiments/220_asr/220_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20280" windowHeight="14260" tabRatio="500"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20280" windowHeight="14265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="27">
   <si>
     <t>Overall performance</t>
   </si>
@@ -101,6 +101,9 @@
   <si>
     <t>SVMCMM VanillaFE</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>all features</t>
   </si>
 </sst>
 </file>
@@ -494,14 +497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:G91"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:G109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -531,7 +534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26">
+    <row r="4" spans="1:7" ht="38.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +557,7 @@
         <v>0.45617021276595698</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26">
+    <row r="5" spans="1:7" ht="25.5">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,7 +580,7 @@
         <v>0.48054919908466798</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26">
+    <row r="6" spans="1:7" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -600,7 +603,7 @@
         <v>0.484969939879759</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26">
+    <row r="7" spans="1:7" ht="25.5">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -623,7 +626,7 @@
         <v>0.50980392156862697</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26">
+    <row r="8" spans="1:7" ht="25.5">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -646,7 +649,7 @@
         <v>0.396039603960396</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26">
+    <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -669,7 +672,7 @@
         <v>0.47495361781076001</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26">
+    <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -692,7 +695,7 @@
         <v>0.48290598290598202</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26">
+    <row r="11" spans="1:7" ht="25.5">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -715,7 +718,7 @@
         <v>0.40816326530612201</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26">
+    <row r="12" spans="1:7" ht="25.5">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -738,7 +741,7 @@
         <v>0.45822102425875999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26">
+    <row r="13" spans="1:7" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -761,7 +764,7 @@
         <v>0.420382165605095</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26">
+    <row r="14" spans="1:7" ht="25.5">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -795,7 +798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="26">
+    <row r="23" spans="1:7" ht="38.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +821,7 @@
         <v>0.483069009858551</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="26">
+    <row r="24" spans="1:7" ht="25.5">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -841,7 +844,7 @@
         <v>0.50655021834061098</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="26">
+    <row r="25" spans="1:7" ht="25.5">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -864,7 +867,7 @@
         <v>0.48728813559321998</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="26">
+    <row r="26" spans="1:7" ht="25.5">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -887,7 +890,7 @@
         <v>0.49305555555555503</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="26">
+    <row r="27" spans="1:7" ht="25.5">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -910,7 +913,7 @@
         <v>0.53405994550408697</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="26">
+    <row r="28" spans="1:7" ht="25.5">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -933,7 +936,7 @@
         <v>0.58051689860834899</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="26">
+    <row r="29" spans="1:7" ht="25.5">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -956,7 +959,7 @@
         <v>0.50185873605947895</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="26">
+    <row r="30" spans="1:7" ht="25.5">
       <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
@@ -979,7 +982,7 @@
         <v>0.51612903225806395</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="26">
+    <row r="31" spans="1:7" ht="25.5">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>0.43859649122806998</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="26">
+    <row r="32" spans="1:7" ht="25.5">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>0.34035087719298202</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="26">
+    <row r="33" spans="1:7" ht="25.5">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="26">
+    <row r="37" spans="1:7" ht="38.25">
       <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>0.12337482710926601</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="26">
+    <row r="38" spans="1:7" ht="25.5">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
@@ -1099,7 +1102,7 @@
         <v>0.158102766798418</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="26">
+    <row r="39" spans="1:7" ht="25.5">
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>9.3617021276595699E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="26">
+    <row r="40" spans="1:7" ht="25.5">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>8.16326530612244E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="26">
+    <row r="41" spans="1:7" ht="25.5">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>9.7165991902833995E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="26">
+    <row r="42" spans="1:7" ht="25.5">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>0.194357366771159</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="26">
+    <row r="43" spans="1:7" ht="25.5">
       <c r="A43" s="1" t="s">
         <v>6</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>0.13114754098360601</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="26">
+    <row r="44" spans="1:7" ht="25.5">
       <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>0.112094395280236</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="26">
+    <row r="45" spans="1:7" ht="25.5">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>0.118251928020565</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="26">
+    <row r="46" spans="1:7" ht="25.5">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>6.4056939501779306E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="26">
+    <row r="47" spans="1:7" ht="25.5">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -1311,7 +1314,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="26">
+    <row r="51" spans="1:7" ht="38.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>0.43667017913593198</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="26">
+    <row r="52" spans="1:7" ht="25.5">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>0.40613026819923298</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="26">
+    <row r="53" spans="1:7" ht="25.5">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>0.45814977973568199</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="26">
+    <row r="54" spans="1:7" ht="25.5">
       <c r="A54" s="1" t="s">
         <v>3</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>0.47173489278752401</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="26">
+    <row r="55" spans="1:7" ht="25.5">
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>0.42495126705653002</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="26">
+    <row r="56" spans="1:7" ht="25.5">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>0.45418326693227001</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="26">
+    <row r="57" spans="1:7" ht="25.5">
       <c r="A57" s="1" t="s">
         <v>6</v>
       </c>
@@ -1472,7 +1475,7 @@
         <v>0.412470023980815</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="26">
+    <row r="58" spans="1:7" ht="25.5">
       <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>0.48275862068965503</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="26">
+    <row r="59" spans="1:7" ht="25.5">
       <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>0.39766081871344999</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="26">
+    <row r="60" spans="1:7" ht="25.5">
       <c r="A60" s="1" t="s">
         <v>9</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>0.39694656488549601</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="26">
+    <row r="61" spans="1:7" ht="25.5">
       <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="26">
+    <row r="67" spans="1:7" ht="38.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>0.41201716738197403</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="26">
+    <row r="68" spans="1:7" ht="25.5">
       <c r="A68" s="1" t="s">
         <v>1</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>0.461928934010152</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="26">
+    <row r="69" spans="1:7" ht="25.5">
       <c r="A69" s="1" t="s">
         <v>2</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>0.38983050847457601</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="26">
+    <row r="70" spans="1:7" ht="25.5">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
@@ -1661,7 +1664,7 @@
         <v>0.46271510516252301</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="26">
+    <row r="71" spans="1:7" ht="25.5">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>0.34825870646766099</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="26">
+    <row r="72" spans="1:7" ht="25.5">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
@@ -1707,7 +1710,7 @@
         <v>0.349881796690307</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="26">
+    <row r="73" spans="1:7" ht="25.5">
       <c r="A73" s="1" t="s">
         <v>6</v>
       </c>
@@ -1730,7 +1733,7 @@
         <v>0.462686567164179</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="26">
+    <row r="74" spans="1:7" ht="25.5">
       <c r="A74" s="1" t="s">
         <v>7</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>0.42777777777777698</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="26">
+    <row r="75" spans="1:7" ht="25.5">
       <c r="A75" s="1" t="s">
         <v>8</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>0.36781609195402298</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="26">
+    <row r="76" spans="1:7" ht="25.5">
       <c r="A76" s="1" t="s">
         <v>9</v>
       </c>
@@ -1799,7 +1802,7 @@
         <v>0.41379310344827502</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="26">
+    <row r="77" spans="1:7" ht="25.5">
       <c r="A77" s="1" t="s">
         <v>10</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="26">
+    <row r="81" spans="1:7" ht="38.25">
       <c r="A81" s="1" t="s">
         <v>0</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>0.39992041384798999</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="26">
+    <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="1" t="s">
         <v>1</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>0.40430107526881698</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="26">
+    <row r="83" spans="1:7" ht="25.5">
       <c r="A83" s="1" t="s">
         <v>2</v>
       </c>
@@ -1896,7 +1899,7 @@
         <v>0.38225255972696198</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="26">
+    <row r="84" spans="1:7" ht="25.5">
       <c r="A84" s="1" t="s">
         <v>3</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>0.41509433962264097</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="26">
+    <row r="85" spans="1:7" ht="25.5">
       <c r="A85" s="1" t="s">
         <v>4</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>0.42857142857142799</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="26">
+    <row r="86" spans="1:7" ht="25.5">
       <c r="A86" s="1" t="s">
         <v>5</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>0.41144901610017798</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="26">
+    <row r="87" spans="1:7" ht="25.5">
       <c r="A87" s="1" t="s">
         <v>6</v>
       </c>
@@ -1988,7 +1991,7 @@
         <v>0.40552995391704999</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="26">
+    <row r="88" spans="1:7" ht="25.5">
       <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>0.375494071146245</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="26">
+    <row r="89" spans="1:7" ht="25.5">
       <c r="A89" s="1" t="s">
         <v>8</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>0.41445783132530101</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="26">
+    <row r="90" spans="1:7" ht="25.5">
       <c r="A90" s="1" t="s">
         <v>9</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>0.39370078740157399</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="26">
+    <row r="91" spans="1:7" ht="25.5">
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
@@ -2078,6 +2081,264 @@
       </c>
       <c r="G91" s="1">
         <v>0.367256637168141</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="38.25">
+      <c r="A99" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="1">
+        <v>0.67342032967032905</v>
+      </c>
+      <c r="C99" s="1">
+        <v>0.40341493519851801</v>
+      </c>
+      <c r="D99" s="1">
+        <v>0.504567091213173</v>
+      </c>
+      <c r="E99" s="1">
+        <v>0.56346255974508697</v>
+      </c>
+      <c r="F99" s="1">
+        <v>0.34993403693931302</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0.43173957273652003</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="25.5">
+      <c r="A100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="1">
+        <v>0.68181818181818099</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0.51724137931034397</v>
+      </c>
+      <c r="E100" s="1">
+        <v>0.51785714285714202</v>
+      </c>
+      <c r="F100" s="1">
+        <v>0.33852140077821002</v>
+      </c>
+      <c r="G100" s="1">
+        <v>0.40941176470588198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="25.5">
+      <c r="A101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="1">
+        <v>0.660377358490566</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0.40887850467289699</v>
+      </c>
+      <c r="D101" s="1">
+        <v>0.50505050505050497</v>
+      </c>
+      <c r="E101" s="1">
+        <v>0.56886227544910095</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0.32423208191126202</v>
+      </c>
+      <c r="G101" s="1">
+        <v>0.41304347826086901</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="25.5">
+      <c r="A102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" s="1">
+        <v>0.64637681159420202</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0.46555323590814102</v>
+      </c>
+      <c r="D102" s="1">
+        <v>0.54126213592232997</v>
+      </c>
+      <c r="E102" s="1">
+        <v>0.58525345622119795</v>
+      </c>
+      <c r="F102" s="1">
+        <v>0.42617449664429502</v>
+      </c>
+      <c r="G102" s="1">
+        <v>0.49320388349514499</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="25.5">
+      <c r="A103" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" s="1">
+        <v>0.74517374517374502</v>
+      </c>
+      <c r="C103" s="1">
+        <v>0.42984409799554502</v>
+      </c>
+      <c r="D103" s="1">
+        <v>0.54519774011299404</v>
+      </c>
+      <c r="E103" s="1">
+        <v>0.61676646706586802</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0.346801346801346</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0.443965517241379</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="25.5">
+      <c r="A104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="1">
+        <v>0.67441860465116199</v>
+      </c>
+      <c r="C104" s="1">
+        <v>0.42116182572614103</v>
+      </c>
+      <c r="D104" s="1">
+        <v>0.51851851851851805</v>
+      </c>
+      <c r="E104" s="1">
+        <v>0.58285714285714196</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0.35789473684210499</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0.44347826086956499</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="25.5">
+      <c r="A105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B105" s="1">
+        <v>0.67741935483870896</v>
+      </c>
+      <c r="C105" s="1">
+        <v>0.37984496124030998</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0.48675496688741698</v>
+      </c>
+      <c r="E105" s="1">
+        <v>0.56291390728476798</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0.37117903930131002</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0.44736842105263103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="25.5">
+      <c r="A106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" s="1">
+        <v>0.71367521367521303</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0.39856801909307799</v>
+      </c>
+      <c r="D106" s="1">
+        <v>0.51148545176110205</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0.56578947368420995</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0.33204633204633199</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0.418491484184914</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="25.5">
+      <c r="A107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0.65107913669064699</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0.36418511066398301</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0.467096774193548</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0.55434782608695599</v>
+      </c>
+      <c r="F107" s="1">
+        <v>0.32903225806451603</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0.41295546558704399</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="25.5">
+      <c r="A108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" s="1">
+        <v>0.64590163934426204</v>
+      </c>
+      <c r="C108" s="1">
+        <v>0.31269841269841198</v>
+      </c>
+      <c r="D108" s="1">
+        <v>0.42139037433155002</v>
+      </c>
+      <c r="E108" s="1">
+        <v>0.53170731707316998</v>
+      </c>
+      <c r="F108" s="1">
+        <v>0.29863013698630098</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0.38245614035087699</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="25.5">
+      <c r="A109" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="1">
+        <v>0.66441441441441396</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0.448328267477203</v>
+      </c>
+      <c r="D109" s="1">
+        <v>0.53539019963702295</v>
+      </c>
+      <c r="E109" s="1">
+        <v>0.55555555555555503</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0.37585421412300601</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0.44836956521739102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>